<commit_message>
Fine Tuning of certain parameters and values
</commit_message>
<xml_diff>
--- a/CC/SRE Kharghar/Auto snag.xlsx
+++ b/CC/SRE Kharghar/Auto snag.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internship\Siemens\CC\SRE Kharghar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46E77A86-0512-458F-B36D-A573C52393A3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6ABDE5DE-4766-409A-9B03-55F83C3EA7F3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="746" xr2:uid="{E331085D-2BF4-414F-ACE7-56B2403B569B}"/>
   </bookViews>
@@ -852,15 +852,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -951,11 +942,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1947,7 +1947,6 @@
       <sheetName val="NewReportDefinition(2)324"/>
       <sheetName val="NewReportDefinition(2)325"/>
       <sheetName val="NewReportDefinition(2)326"/>
-      <sheetName val="Kharghar"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -2160,10 +2159,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
       <sheetData sheetId="34">
         <row r="4">
           <cell r="D4">
@@ -2227,9 +2226,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
       <sheetData sheetId="46">
         <row r="4">
           <cell r="D4">
@@ -2293,10 +2292,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
       <sheetData sheetId="59">
         <row r="4">
           <cell r="D4">
@@ -2354,10 +2353,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-      <sheetData sheetId="71" refreshError="1"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
       <sheetData sheetId="72">
         <row r="4">
           <cell r="D4">
@@ -2421,10 +2420,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="81" refreshError="1"/>
-      <sheetData sheetId="82" refreshError="1"/>
-      <sheetData sheetId="83" refreshError="1"/>
-      <sheetData sheetId="84" refreshError="1"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
       <sheetData sheetId="85">
         <row r="4">
           <cell r="D4">
@@ -2488,10 +2487,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="94" refreshError="1"/>
-      <sheetData sheetId="95" refreshError="1"/>
-      <sheetData sheetId="96" refreshError="1"/>
-      <sheetData sheetId="97" refreshError="1"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
       <sheetData sheetId="98">
         <row r="4">
           <cell r="D4">
@@ -2605,7 +2604,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="115" refreshError="1"/>
+      <sheetData sheetId="115"/>
       <sheetData sheetId="116">
         <row r="4">
           <cell r="D4">
@@ -2620,7 +2619,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="118" refreshError="1"/>
+      <sheetData sheetId="118"/>
       <sheetData sheetId="119">
         <row r="4">
           <cell r="D4">
@@ -2656,7 +2655,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="124" refreshError="1"/>
+      <sheetData sheetId="124"/>
       <sheetData sheetId="125">
         <row r="4">
           <cell r="D4">
@@ -3014,7 +3013,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="176" refreshError="1"/>
+      <sheetData sheetId="176"/>
       <sheetData sheetId="177">
         <row r="4">
           <cell r="D4">
@@ -3485,32 +3484,32 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="245" refreshError="1"/>
-      <sheetData sheetId="246" refreshError="1"/>
-      <sheetData sheetId="247" refreshError="1"/>
-      <sheetData sheetId="248" refreshError="1"/>
-      <sheetData sheetId="249" refreshError="1"/>
-      <sheetData sheetId="250" refreshError="1"/>
-      <sheetData sheetId="251" refreshError="1"/>
-      <sheetData sheetId="252" refreshError="1"/>
-      <sheetData sheetId="253" refreshError="1"/>
-      <sheetData sheetId="254" refreshError="1"/>
-      <sheetData sheetId="255" refreshError="1"/>
-      <sheetData sheetId="256" refreshError="1"/>
-      <sheetData sheetId="257" refreshError="1"/>
-      <sheetData sheetId="258" refreshError="1"/>
-      <sheetData sheetId="259" refreshError="1"/>
-      <sheetData sheetId="260" refreshError="1"/>
-      <sheetData sheetId="261" refreshError="1"/>
-      <sheetData sheetId="262" refreshError="1"/>
-      <sheetData sheetId="263" refreshError="1"/>
-      <sheetData sheetId="264" refreshError="1"/>
-      <sheetData sheetId="265" refreshError="1"/>
-      <sheetData sheetId="266" refreshError="1"/>
-      <sheetData sheetId="267" refreshError="1"/>
-      <sheetData sheetId="268" refreshError="1"/>
-      <sheetData sheetId="269" refreshError="1"/>
-      <sheetData sheetId="270" refreshError="1"/>
+      <sheetData sheetId="245"/>
+      <sheetData sheetId="246"/>
+      <sheetData sheetId="247"/>
+      <sheetData sheetId="248"/>
+      <sheetData sheetId="249"/>
+      <sheetData sheetId="250"/>
+      <sheetData sheetId="251"/>
+      <sheetData sheetId="252"/>
+      <sheetData sheetId="253"/>
+      <sheetData sheetId="254"/>
+      <sheetData sheetId="255"/>
+      <sheetData sheetId="256"/>
+      <sheetData sheetId="257"/>
+      <sheetData sheetId="258"/>
+      <sheetData sheetId="259"/>
+      <sheetData sheetId="260"/>
+      <sheetData sheetId="261"/>
+      <sheetData sheetId="262"/>
+      <sheetData sheetId="263"/>
+      <sheetData sheetId="264"/>
+      <sheetData sheetId="265"/>
+      <sheetData sheetId="266"/>
+      <sheetData sheetId="267"/>
+      <sheetData sheetId="268"/>
+      <sheetData sheetId="269"/>
+      <sheetData sheetId="270"/>
       <sheetData sheetId="271">
         <row r="4">
           <cell r="D4">
@@ -3602,7 +3601,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="284" refreshError="1"/>
+      <sheetData sheetId="284"/>
       <sheetData sheetId="285">
         <row r="4">
           <cell r="D4">
@@ -3610,7 +3609,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="286" refreshError="1"/>
+      <sheetData sheetId="286"/>
       <sheetData sheetId="287">
         <row r="4">
           <cell r="D4">
@@ -3843,7 +3842,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="327" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4152,7 +4150,7 @@
   <dimension ref="A1:BV7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,7 +4167,8 @@
     <col min="10" max="10" width="8.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="17" width="14" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
     <col min="18" max="18" width="17.7109375" customWidth="1"/>
     <col min="19" max="19" width="13.140625" customWidth="1"/>
     <col min="20" max="20" width="15.140625" customWidth="1"/>
@@ -4178,70 +4177,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="31" t="s">
         <v>14</v>
       </c>
       <c r="W1" s="4"/>
@@ -4298,7 +4297,7 @@
       <c r="BV1" s="4"/>
     </row>
     <row r="2" spans="1:74" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="59" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -4355,11 +4354,11 @@
         <f>'[1]NewReportDefinition(2)34'!$D$4</f>
         <v>50</v>
       </c>
-      <c r="P2" s="22">
-        <f>IF(L2&lt;M2,0,IF(M2-L2&gt;250,50,IF(M2-L2&gt;200,30,25)))</f>
+      <c r="P2" s="17">
+        <f>IF(L2-M2&lt;-150,0,IF(L2-M2&lt;0,20,IF(L2-M2&lt;151,(2/15)*(L2-M2)+20,IF(L2-M2&lt;201,(19/49)*(L2-M2)-(860/49),IF(L2-M2&lt;250,(19/49)*(L2-M2)-(830/49),100)))))</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="17" t="str">
+      <c r="Q2" s="11" t="str">
         <f>IF(EXACT(O2,P2),"OK","FAULT")</f>
         <v>FAULT</v>
       </c>
@@ -4385,7 +4384,7 @@
       </c>
     </row>
     <row r="3" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="20" t="s">
         <v>54</v>
       </c>
@@ -4440,11 +4439,11 @@
         <f>'[1]NewReportDefinition(2)46'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="P3" s="23">
-        <f t="shared" ref="P3:P7" si="6">IF(L3&lt;M3,0,IF(M3-L3&gt;250,50,IF(M3-L3&gt;200,30,25)))</f>
-        <v>25</v>
-      </c>
-      <c r="Q3" s="18" t="str">
+      <c r="P3" s="18">
+        <f t="shared" ref="P3:P7" si="6">IF(L3-M3&lt;-150,0,IF(L3-M3&lt;0,20,IF(L3-M3&lt;151,(2/15)*(L3-M3)+20,IF(L3-M3&lt;201,(19/49)*(L3-M3)-(860/49),IF(L3-M3&lt;250,(19/49)*(L3-M3)-(830/49),100)))))</f>
+        <v>25.120003255208395</v>
+      </c>
+      <c r="Q3" s="12" t="str">
         <f t="shared" ref="Q3:Q7" si="7">IF(EXACT(O3,P3),"OK","FAULT")</f>
         <v>FAULT</v>
       </c>
@@ -4470,7 +4469,7 @@
       </c>
     </row>
     <row r="4" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="20" t="s">
         <v>55</v>
       </c>
@@ -4525,11 +4524,11 @@
         <f>'[1]NewReportDefinition(2)59'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="18">
         <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="Q4" s="18" t="str">
+        <v>39.021329752604132</v>
+      </c>
+      <c r="Q4" s="12" t="str">
         <f t="shared" si="7"/>
         <v>FAULT</v>
       </c>
@@ -4555,7 +4554,7 @@
       </c>
     </row>
     <row r="5" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="20" t="s">
         <v>56</v>
       </c>
@@ -4610,13 +4609,13 @@
         <f>'[1]NewReportDefinition(2)72'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="18" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>OK</v>
+        <v>FAULT</v>
       </c>
       <c r="R5" s="2">
         <f>'[1]NewReportDefinition(2)65'!$D$4</f>
@@ -4640,7 +4639,7 @@
       </c>
     </row>
     <row r="6" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="21" t="s">
         <v>57</v>
       </c>
@@ -4695,11 +4694,11 @@
         <f>'[1]NewReportDefinition(2)85'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="18">
         <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="Q6" s="18" t="str">
+        <v>30.053336588541725</v>
+      </c>
+      <c r="Q6" s="12" t="str">
         <f t="shared" si="7"/>
         <v>FAULT</v>
       </c>
@@ -4725,7 +4724,7 @@
       </c>
     </row>
     <row r="7" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="20" t="s">
         <v>58</v>
       </c>
@@ -4780,11 +4779,11 @@
         <f>'[1]NewReportDefinition(2)98'!$D$4</f>
         <v>50</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="19">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="19" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="13" t="str">
         <f t="shared" si="7"/>
         <v>FAULT</v>
       </c>
@@ -5010,18 +5009,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="7">
@@ -5034,7 +5033,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="53" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="7">
@@ -5047,7 +5046,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="42" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="7">
@@ -5060,7 +5059,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="53" t="s">
         <v>102</v>
       </c>
       <c r="B5" s="7">
@@ -5073,7 +5072,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="42" t="s">
         <v>103</v>
       </c>
       <c r="B6" s="7">
@@ -5086,7 +5085,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="53" t="s">
         <v>104</v>
       </c>
       <c r="B7" s="7">
@@ -5099,7 +5098,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="42" t="s">
         <v>105</v>
       </c>
       <c r="B8" s="7">
@@ -5112,7 +5111,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="53" t="s">
         <v>106</v>
       </c>
       <c r="B9" s="7">
@@ -5125,7 +5124,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="42" t="s">
         <v>107</v>
       </c>
       <c r="B10" s="7">
@@ -5138,7 +5137,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="53" t="s">
         <v>108</v>
       </c>
       <c r="B11" s="7">
@@ -5151,7 +5150,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="42" t="s">
         <v>109</v>
       </c>
       <c r="B12" s="7">
@@ -5164,7 +5163,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="53" t="s">
         <v>110</v>
       </c>
       <c r="B13" s="7">
@@ -5177,7 +5176,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="42" t="s">
         <v>111</v>
       </c>
       <c r="B14" s="7">
@@ -5190,7 +5189,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="53" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="7">
@@ -5203,7 +5202,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="42" t="s">
         <v>113</v>
       </c>
       <c r="B16" s="7">
@@ -5216,7 +5215,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="53" t="s">
         <v>114</v>
       </c>
       <c r="B17" s="7">
@@ -5229,7 +5228,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="42" t="s">
         <v>115</v>
       </c>
       <c r="B18" s="7">
@@ -5242,7 +5241,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="53" t="s">
         <v>116</v>
       </c>
       <c r="B19" s="7">
@@ -5255,7 +5254,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="42" t="s">
         <v>117</v>
       </c>
       <c r="B20" s="7">
@@ -5268,7 +5267,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="53" t="s">
         <v>119</v>
       </c>
       <c r="B21" s="7">
@@ -5281,7 +5280,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="42" t="s">
         <v>120</v>
       </c>
       <c r="B22" s="7">
@@ -5294,7 +5293,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="53" t="s">
         <v>121</v>
       </c>
       <c r="B23" s="7">
@@ -5307,7 +5306,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="42" t="s">
         <v>122</v>
       </c>
       <c r="B24" s="7">
@@ -5320,7 +5319,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="53" t="s">
         <v>123</v>
       </c>
       <c r="B25" s="7">
@@ -5333,7 +5332,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="42" t="s">
         <v>124</v>
       </c>
       <c r="B26" s="7">
@@ -5346,7 +5345,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="53" t="s">
         <v>125</v>
       </c>
       <c r="B27" s="7">
@@ -5359,7 +5358,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="42" t="s">
         <v>126</v>
       </c>
       <c r="B28" s="7">
@@ -5372,7 +5371,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="45" t="s">
         <v>127</v>
       </c>
       <c r="B29" s="10">
@@ -5395,7 +5394,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5413,39 +5412,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="39" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="9" t="str">
@@ -5533,252 +5532,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="34" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="38" t="str">
+      <c r="B2" s="35" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)0'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39" t="str">
+      <c r="B3" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)1'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="39" t="str">
+      <c r="B4" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)2'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="39" t="str">
+      <c r="B5" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)3'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="39" t="str">
+      <c r="B6" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)4'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="39" t="str">
+      <c r="B7" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)5'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="39" t="str">
+      <c r="B8" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)6'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="39" t="str">
+      <c r="B9" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)7'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="39" t="str">
+      <c r="B10" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)8'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="39" t="str">
+      <c r="B11" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)9'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="39" t="str">
+      <c r="B12" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)10'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="39" t="str">
+      <c r="B13" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)11'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="39" t="str">
+      <c r="B14" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)12'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="39" t="str">
+      <c r="B15" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)13'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="39" t="str">
+      <c r="B16" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)14'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="39" t="str">
+      <c r="B17" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)15'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="39" t="str">
+      <c r="B18" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)16'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="39" t="str">
+      <c r="B19" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)17'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="39" t="str">
+      <c r="B20" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)18'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="39" t="str">
+      <c r="B21" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)19'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="39" t="str">
+      <c r="B22" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)20'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="39" t="str">
+      <c r="B23" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)21'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="39" t="str">
+      <c r="B24" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)22'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="39" t="str">
+      <c r="B25" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)23'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="39" t="str">
+      <c r="B26" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)24'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="39" t="str">
+      <c r="B27" s="36" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)25'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="40" t="str">
+      <c r="B28" s="37" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)26'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
@@ -5801,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1379126D-3CF7-456C-A76F-4E2D319EEB2B}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5818,126 +5817,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="46" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)136'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="C2" s="27" t="str">
+      <c r="C2" s="24" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)137'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="D2" s="27" t="str">
+      <c r="D2" s="24" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)138'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="E2" s="27" t="str">
+      <c r="E2" s="24" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)139'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="F2" s="27" t="str">
+      <c r="F2" s="24" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)140'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="24">
         <f>'[1]NewReportDefinition(2)141'!$D$4</f>
         <v>42.369998931884801</v>
       </c>
-      <c r="H2" s="50">
+      <c r="H2" s="47">
         <f>'[1]NewReportDefinition(2)142'!$D$4</f>
         <v>31.4899997711182</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="46" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)143'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="C3" s="51" t="str">
+      <c r="C3" s="48" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)144'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="D3" s="51" t="str">
+      <c r="D3" s="48" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)145'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="E3" s="51" t="str">
+      <c r="E3" s="48" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)146'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="F3" s="51" t="str">
+      <c r="F3" s="48" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)147'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="48">
         <f>'[1]NewReportDefinition(2)148'!$D$4</f>
         <v>42.239997863769503</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="47">
         <f>'[1]NewReportDefinition(2)149'!$D$4</f>
         <v>31.5399990081787</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="52" t="str">
+      <c r="B4" s="49" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)150'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="C4" s="53" t="str">
+      <c r="C4" s="50" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)151'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="D4" s="53" t="str">
+      <c r="D4" s="50" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)152'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="E4" s="53" t="str">
+      <c r="E4" s="50" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)153'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="F4" s="53" t="str">
+      <c r="F4" s="50" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)154'!$D$4,"0"),"OFF","ON")</f>
         <v>ON</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="50">
         <f>'[1]NewReportDefinition(2)155'!$D$4</f>
         <v>43.450000762939503</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="51">
         <f>'[1]NewReportDefinition(2)156'!$D$4</f>
         <v>33.200000762939503</v>
       </c>
@@ -5968,7 +5967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478D22E1-34A6-4DAC-8B34-2B2576F5F5C6}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -5992,60 +5991,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="39" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>85</v>
       </c>
       <c r="B2" s="11" t="str">
@@ -6114,7 +6113,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="52" t="s">
         <v>101</v>
       </c>
       <c r="B3" s="13" t="str">
@@ -6200,7 +6199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92119663-30D8-4932-82BE-DD028DE1E53A}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -6215,197 +6214,197 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="39" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="25">
         <f>'[1]NewReportDefinition(2)291'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <f>'[1]NewReportDefinition(2)295'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="25">
         <f>'[1]NewReportDefinition(2)299'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="26">
         <f>'[1]NewReportDefinition(2)303'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <f>'[1]NewReportDefinition(2)307'!$D$4</f>
         <v>575</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="26">
         <f>'[1]NewReportDefinition(2)311'!$D$4</f>
         <v>3457</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="25">
         <f>'[1]NewReportDefinition(2)315'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="I2" s="29" t="str">
+      <c r="I2" s="26" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)319'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="27">
         <f>'[1]NewReportDefinition(2)323'!$D$4</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="25">
         <f>'[1]NewReportDefinition(2)292'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="26">
         <f>'[1]NewReportDefinition(2)296'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="25">
         <f>'[1]NewReportDefinition(2)300'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="26">
         <f>'[1]NewReportDefinition(2)304'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="25">
         <f>'[1]NewReportDefinition(2)308'!$D$4</f>
         <v>579</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="26">
         <f>'[1]NewReportDefinition(2)312'!$D$4</f>
         <v>3599</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="25">
         <f>'[1]NewReportDefinition(2)316'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="I3" s="29" t="str">
+      <c r="I3" s="26" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)320'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="27">
         <f>'[1]NewReportDefinition(2)324'!$D$4</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="25">
         <f>[1]!Table285[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="26">
         <f>[1]!Table289[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="25">
         <f>[1]!Table293[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <f>[1]!Table297[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <f>[1]!Table301[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="26">
         <f>[1]!Table305[[#This Row],[Value]]</f>
         <v>3243</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="25">
         <f>[1]!Table309[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
-      <c r="I4" s="29" t="str">
+      <c r="I4" s="26" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)321'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="27">
         <f>[1]!Table317[[#This Row],[Value]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="28">
         <f>'[1]NewReportDefinition(2)294'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <f>'[1]NewReportDefinition(2)298'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="28">
         <f>'[1]NewReportDefinition(2)302'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="29">
         <f>'[1]NewReportDefinition(2)306'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="28">
         <f>'[1]NewReportDefinition(2)310'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="29">
         <f>'[1]NewReportDefinition(2)314'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="28">
         <f>'[1]NewReportDefinition(2)318'!$D$4</f>
         <v>0</v>
       </c>
-      <c r="I5" s="32" t="str">
+      <c r="I5" s="29" t="str">
         <f>IF(EXACT('[1]NewReportDefinition(2)322'!$D$4,"0"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="30">
         <f>'[1]NewReportDefinition(2)326'!$D$4</f>
         <v>0</v>
       </c>
@@ -6428,8 +6427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49AFFE8-DDE8-455C-9F36-C2A7F98D2DA8}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6443,16 +6442,16 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>143</v>
       </c>
       <c r="F1" s="1"/>
@@ -6461,10 +6460,10 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="31" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="12" t="str">
@@ -6485,8 +6484,8 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="31" t="s">
         <v>141</v>
       </c>
       <c r="C3" s="12" t="str">
@@ -6507,8 +6506,8 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="55" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="58" t="s">
         <v>142</v>
       </c>
       <c r="C4" s="13" t="str">
@@ -6631,7 +6630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05665607-FB58-4358-B111-9F3B9347FBE3}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -6642,18 +6641,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="4" t="str">
@@ -6666,7 +6665,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="9" t="str">
@@ -6696,7 +6695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B10017A-5B65-48BF-A738-0AA429FBC156}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6713,33 +6712,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="4" t="str">
@@ -6772,7 +6771,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="4" t="str">
@@ -6805,7 +6804,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="45" t="s">
         <v>67</v>
       </c>
       <c r="B4" s="9" t="str">
@@ -6880,7 +6879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A81E2D-400D-41F2-8757-141426B71285}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6894,27 +6893,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="42" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="4" t="str">
@@ -6939,7 +6938,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="45" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="9" t="str">

</xml_diff>